<commit_message>
Working on project (HPC, Gantt, Path changes to files, logbook)
</commit_message>
<xml_diff>
--- a/Gantt_chart.xlsx
+++ b/Gantt_chart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\henri\Documents\Git\Git_Projects\Classifier_Guided_Diffusion_for_Point_Clouds-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{262269FE-054B-4AED-9AFD-141A7EA2A9EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AE3778C-5765-45A9-867E-62D630CA4C9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22046" yWindow="-2177" windowWidth="22149" windowHeight="13200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2430" yWindow="3375" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project schedule" sheetId="11" r:id="rId1"/>
@@ -1117,19 +1117,30 @@
     <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="167" fontId="16" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="167" fontId="16" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="166" fontId="22" fillId="0" borderId="0" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="167" fontId="16" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="167" fontId="16" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="16" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="16" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="3" applyAlignment="1">
@@ -1144,19 +1155,8 @@
     <xf numFmtId="0" fontId="17" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="22" fillId="0" borderId="0" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="167" fontId="16" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -1174,224 +1174,17 @@
     <cellStyle name="Title" xfId="5" builtinId="15" customBuiltin="1"/>
     <cellStyle name="zHiddenText" xfId="3" xr:uid="{26E66EE6-E33F-4D77-BAE4-0FB4F5BBF673}"/>
   </cellStyles>
-  <dxfs count="53">
+  <dxfs count="30">
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
       <border>
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="0" tint="-4.9989318521683403E-2"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-4.9989318521683403E-2"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="0" tint="-4.9989318521683403E-2"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-4.9989318521683403E-2"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="0" tint="-4.9989318521683403E-2"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-4.9989318521683403E-2"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="0" tint="-4.9989318521683403E-2"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-4.9989318521683403E-2"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="0" tint="-4.9989318521683403E-2"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-4.9989318521683403E-2"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="0" tint="-4.9989318521683403E-2"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-4.9989318521683403E-2"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="0" tint="-4.9989318521683403E-2"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-4.9989318521683403E-2"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="0" tint="-4.9989318521683403E-2"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-4.9989318521683403E-2"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="0" tint="-4.9989318521683403E-2"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-4.9989318521683403E-2"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="0" tint="-4.9989318521683403E-2"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-4.9989318521683403E-2"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="0" tint="-4.9989318521683403E-2"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-4.9989318521683403E-2"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="0" tint="-4.9989318521683403E-2"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-4.9989318521683403E-2"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
+        <left style="thin">
+          <color theme="5"/>
+        </left>
+        <right style="thin">
+          <color theme="5"/>
+        </right>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1419,18 +1212,22 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
       <border>
-        <left/>
-        <right/>
+        <top style="thin">
+          <color theme="0" tint="-4.9989318521683403E-2"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-4.9989318521683403E-2"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
+          <bgColor theme="6" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
       <border>
@@ -1479,42 +1276,19 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
-      <border>
-        <top style="thin">
-          <color theme="0" tint="-4.9989318521683403E-2"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-4.9989318521683403E-2"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
+          <bgColor theme="5" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
       <border>
         <left/>
         <right/>
-        <top style="thin">
-          <color theme="0" tint="-4.9989318521683403E-2"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-4.9989318521683403E-2"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
         <top style="thin">
           <color theme="0" tint="-4.9989318521683403E-2"/>
         </top>
@@ -1631,13 +1405,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="4" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
@@ -1655,10 +1422,12 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
       <border>
+        <left/>
+        <right/>
         <top style="thin">
           <color theme="0" tint="-4.9989318521683403E-2"/>
         </top>
@@ -1682,46 +1451,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="8"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="0" tint="-4.9989318521683403E-2"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-4.9989318521683403E-2"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
       <border>
@@ -1732,30 +1462,6 @@
           <color theme="0" tint="-4.9989318521683403E-2"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="0" tint="-4.9989318521683403E-2"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-4.9989318521683403E-2"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -1772,33 +1478,6 @@
         <bottom style="thin">
           <color theme="0" tint="-4.9989318521683403E-2"/>
         </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="0" tint="-4.9989318521683403E-2"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-4.9989318521683403E-2"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="5"/>
-        </left>
-        <right style="thin">
-          <color theme="5"/>
-        </right>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1897,15 +1576,15 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="ToDoList" pivot="0" count="9" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="52"/>
-      <tableStyleElement type="headerRow" dxfId="51"/>
-      <tableStyleElement type="totalRow" dxfId="50"/>
-      <tableStyleElement type="firstColumn" dxfId="49"/>
-      <tableStyleElement type="lastColumn" dxfId="48"/>
-      <tableStyleElement type="firstRowStripe" dxfId="47"/>
-      <tableStyleElement type="secondRowStripe" dxfId="46"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="45"/>
-      <tableStyleElement type="secondColumnStripe" dxfId="44"/>
+      <tableStyleElement type="wholeTable" dxfId="29"/>
+      <tableStyleElement type="headerRow" dxfId="28"/>
+      <tableStyleElement type="totalRow" dxfId="27"/>
+      <tableStyleElement type="firstColumn" dxfId="26"/>
+      <tableStyleElement type="lastColumn" dxfId="25"/>
+      <tableStyleElement type="firstRowStripe" dxfId="24"/>
+      <tableStyleElement type="secondRowStripe" dxfId="23"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="22"/>
+      <tableStyleElement type="secondColumnStripe" dxfId="21"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -2262,8 +1941,8 @@
   </sheetPr>
   <dimension ref="A1:FF74"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="B43" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="B67" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2323,28 +2002,28 @@
       <c r="E1" s="15"/>
       <c r="F1" s="16"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="103" t="s">
+      <c r="I1" s="96" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="103"/>
-      <c r="K1" s="103"/>
-      <c r="L1" s="103"/>
-      <c r="M1" s="103"/>
-      <c r="N1" s="103"/>
-      <c r="O1" s="103"/>
+      <c r="J1" s="96"/>
+      <c r="K1" s="96"/>
+      <c r="L1" s="96"/>
+      <c r="M1" s="96"/>
+      <c r="N1" s="96"/>
+      <c r="O1" s="96"/>
       <c r="P1" s="19"/>
-      <c r="Q1" s="102">
+      <c r="Q1" s="95">
         <v>45329</v>
       </c>
-      <c r="R1" s="101"/>
-      <c r="S1" s="101"/>
-      <c r="T1" s="101"/>
-      <c r="U1" s="101"/>
-      <c r="V1" s="101"/>
-      <c r="W1" s="101"/>
-      <c r="X1" s="101"/>
-      <c r="Y1" s="101"/>
-      <c r="Z1" s="101"/>
+      <c r="R1" s="94"/>
+      <c r="S1" s="94"/>
+      <c r="T1" s="94"/>
+      <c r="U1" s="94"/>
+      <c r="V1" s="94"/>
+      <c r="W1" s="94"/>
+      <c r="X1" s="94"/>
+      <c r="Y1" s="94"/>
+      <c r="Z1" s="94"/>
     </row>
     <row r="2" spans="1:162" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B2" s="75" t="s">
@@ -2354,26 +2033,26 @@
       <c r="D2" s="17"/>
       <c r="E2" s="18"/>
       <c r="F2" s="17"/>
-      <c r="I2" s="103" t="s">
+      <c r="I2" s="96" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="103"/>
-      <c r="K2" s="103"/>
-      <c r="L2" s="103"/>
-      <c r="M2" s="103"/>
-      <c r="N2" s="103"/>
-      <c r="O2" s="103"/>
+      <c r="J2" s="96"/>
+      <c r="K2" s="96"/>
+      <c r="L2" s="96"/>
+      <c r="M2" s="96"/>
+      <c r="N2" s="96"/>
+      <c r="O2" s="96"/>
       <c r="P2" s="19"/>
-      <c r="Q2" s="100"/>
-      <c r="R2" s="101"/>
-      <c r="S2" s="101"/>
-      <c r="T2" s="101"/>
-      <c r="U2" s="101"/>
-      <c r="V2" s="101"/>
-      <c r="W2" s="101"/>
-      <c r="X2" s="101"/>
-      <c r="Y2" s="101"/>
-      <c r="Z2" s="101"/>
+      <c r="Q2" s="93"/>
+      <c r="R2" s="94"/>
+      <c r="S2" s="94"/>
+      <c r="T2" s="94"/>
+      <c r="U2" s="94"/>
+      <c r="V2" s="94"/>
+      <c r="W2" s="94"/>
+      <c r="X2" s="94"/>
+      <c r="Y2" s="94"/>
+      <c r="Z2" s="94"/>
     </row>
     <row r="3" spans="1:162" s="20" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="10"/>
@@ -2387,242 +2066,242 @@
       <c r="A4" s="11"/>
       <c r="B4" s="23"/>
       <c r="E4" s="24"/>
-      <c r="I4" s="90">
+      <c r="I4" s="97">
         <f>I5</f>
         <v>45320</v>
       </c>
-      <c r="J4" s="90"/>
-      <c r="K4" s="90"/>
-      <c r="L4" s="90"/>
-      <c r="M4" s="90"/>
-      <c r="N4" s="90"/>
-      <c r="O4" s="91"/>
-      <c r="P4" s="92">
+      <c r="J4" s="97"/>
+      <c r="K4" s="97"/>
+      <c r="L4" s="97"/>
+      <c r="M4" s="97"/>
+      <c r="N4" s="97"/>
+      <c r="O4" s="98"/>
+      <c r="P4" s="89">
         <f>P5</f>
         <v>45327</v>
       </c>
-      <c r="Q4" s="92"/>
-      <c r="R4" s="92"/>
-      <c r="S4" s="92"/>
-      <c r="T4" s="92"/>
-      <c r="U4" s="92"/>
-      <c r="V4" s="92"/>
-      <c r="W4" s="92">
+      <c r="Q4" s="89"/>
+      <c r="R4" s="89"/>
+      <c r="S4" s="89"/>
+      <c r="T4" s="89"/>
+      <c r="U4" s="89"/>
+      <c r="V4" s="89"/>
+      <c r="W4" s="89">
         <f>W5</f>
         <v>45334</v>
       </c>
-      <c r="X4" s="92"/>
-      <c r="Y4" s="92"/>
-      <c r="Z4" s="92"/>
-      <c r="AA4" s="92"/>
-      <c r="AB4" s="92"/>
-      <c r="AC4" s="92"/>
-      <c r="AD4" s="92">
+      <c r="X4" s="89"/>
+      <c r="Y4" s="89"/>
+      <c r="Z4" s="89"/>
+      <c r="AA4" s="89"/>
+      <c r="AB4" s="89"/>
+      <c r="AC4" s="89"/>
+      <c r="AD4" s="89">
         <f>AD5</f>
         <v>45341</v>
       </c>
-      <c r="AE4" s="92"/>
-      <c r="AF4" s="92"/>
-      <c r="AG4" s="92"/>
-      <c r="AH4" s="92"/>
-      <c r="AI4" s="92"/>
-      <c r="AJ4" s="92"/>
-      <c r="AK4" s="92">
+      <c r="AE4" s="89"/>
+      <c r="AF4" s="89"/>
+      <c r="AG4" s="89"/>
+      <c r="AH4" s="89"/>
+      <c r="AI4" s="89"/>
+      <c r="AJ4" s="89"/>
+      <c r="AK4" s="89">
         <f>AK5</f>
         <v>45348</v>
       </c>
-      <c r="AL4" s="92"/>
-      <c r="AM4" s="92"/>
-      <c r="AN4" s="92"/>
-      <c r="AO4" s="92"/>
-      <c r="AP4" s="92"/>
-      <c r="AQ4" s="92"/>
-      <c r="AR4" s="92">
+      <c r="AL4" s="89"/>
+      <c r="AM4" s="89"/>
+      <c r="AN4" s="89"/>
+      <c r="AO4" s="89"/>
+      <c r="AP4" s="89"/>
+      <c r="AQ4" s="89"/>
+      <c r="AR4" s="89">
         <f>AR5</f>
         <v>45355</v>
       </c>
-      <c r="AS4" s="92"/>
-      <c r="AT4" s="92"/>
-      <c r="AU4" s="92"/>
-      <c r="AV4" s="92"/>
-      <c r="AW4" s="92"/>
-      <c r="AX4" s="92"/>
-      <c r="AY4" s="92">
+      <c r="AS4" s="89"/>
+      <c r="AT4" s="89"/>
+      <c r="AU4" s="89"/>
+      <c r="AV4" s="89"/>
+      <c r="AW4" s="89"/>
+      <c r="AX4" s="89"/>
+      <c r="AY4" s="89">
         <f>AY5</f>
         <v>45362</v>
       </c>
-      <c r="AZ4" s="92"/>
-      <c r="BA4" s="92"/>
-      <c r="BB4" s="92"/>
-      <c r="BC4" s="92"/>
-      <c r="BD4" s="92"/>
-      <c r="BE4" s="92"/>
-      <c r="BF4" s="92">
+      <c r="AZ4" s="89"/>
+      <c r="BA4" s="89"/>
+      <c r="BB4" s="89"/>
+      <c r="BC4" s="89"/>
+      <c r="BD4" s="89"/>
+      <c r="BE4" s="89"/>
+      <c r="BF4" s="89">
         <f>BF5</f>
         <v>45369</v>
       </c>
-      <c r="BG4" s="92"/>
-      <c r="BH4" s="92"/>
-      <c r="BI4" s="92"/>
-      <c r="BJ4" s="92"/>
-      <c r="BK4" s="92"/>
-      <c r="BL4" s="89"/>
-      <c r="BM4" s="91">
+      <c r="BG4" s="89"/>
+      <c r="BH4" s="89"/>
+      <c r="BI4" s="89"/>
+      <c r="BJ4" s="89"/>
+      <c r="BK4" s="89"/>
+      <c r="BL4" s="90"/>
+      <c r="BM4" s="98">
         <f>BM5</f>
         <v>45376</v>
       </c>
-      <c r="BN4" s="92"/>
-      <c r="BO4" s="92"/>
-      <c r="BP4" s="92"/>
-      <c r="BQ4" s="92"/>
-      <c r="BR4" s="92"/>
-      <c r="BS4" s="92"/>
-      <c r="BT4" s="92">
+      <c r="BN4" s="89"/>
+      <c r="BO4" s="89"/>
+      <c r="BP4" s="89"/>
+      <c r="BQ4" s="89"/>
+      <c r="BR4" s="89"/>
+      <c r="BS4" s="89"/>
+      <c r="BT4" s="89">
         <f>BT5</f>
         <v>45383</v>
       </c>
-      <c r="BU4" s="92"/>
-      <c r="BV4" s="92"/>
-      <c r="BW4" s="92"/>
-      <c r="BX4" s="92"/>
-      <c r="BY4" s="92"/>
-      <c r="BZ4" s="92"/>
-      <c r="CA4" s="92">
+      <c r="BU4" s="89"/>
+      <c r="BV4" s="89"/>
+      <c r="BW4" s="89"/>
+      <c r="BX4" s="89"/>
+      <c r="BY4" s="89"/>
+      <c r="BZ4" s="89"/>
+      <c r="CA4" s="89">
         <f>CA5</f>
         <v>45390</v>
       </c>
-      <c r="CB4" s="92"/>
-      <c r="CC4" s="92"/>
-      <c r="CD4" s="92"/>
-      <c r="CE4" s="92"/>
-      <c r="CF4" s="92"/>
-      <c r="CG4" s="92"/>
-      <c r="CH4" s="92">
+      <c r="CB4" s="89"/>
+      <c r="CC4" s="89"/>
+      <c r="CD4" s="89"/>
+      <c r="CE4" s="89"/>
+      <c r="CF4" s="89"/>
+      <c r="CG4" s="89"/>
+      <c r="CH4" s="89">
         <f>CH5</f>
         <v>45397</v>
       </c>
-      <c r="CI4" s="92"/>
-      <c r="CJ4" s="93"/>
-      <c r="CK4" s="92"/>
-      <c r="CL4" s="92"/>
-      <c r="CM4" s="92"/>
-      <c r="CN4" s="92"/>
-      <c r="CO4" s="92">
+      <c r="CI4" s="89"/>
+      <c r="CJ4" s="103"/>
+      <c r="CK4" s="89"/>
+      <c r="CL4" s="89"/>
+      <c r="CM4" s="89"/>
+      <c r="CN4" s="89"/>
+      <c r="CO4" s="89">
         <f>CO5</f>
         <v>45404</v>
       </c>
-      <c r="CP4" s="92"/>
-      <c r="CQ4" s="92"/>
-      <c r="CR4" s="92"/>
-      <c r="CS4" s="92"/>
-      <c r="CT4" s="92"/>
-      <c r="CU4" s="92"/>
-      <c r="CV4" s="92">
+      <c r="CP4" s="89"/>
+      <c r="CQ4" s="89"/>
+      <c r="CR4" s="89"/>
+      <c r="CS4" s="89"/>
+      <c r="CT4" s="89"/>
+      <c r="CU4" s="89"/>
+      <c r="CV4" s="89">
         <f>CV5</f>
         <v>45411</v>
       </c>
-      <c r="CW4" s="92"/>
-      <c r="CX4" s="92"/>
-      <c r="CY4" s="92"/>
-      <c r="CZ4" s="92"/>
-      <c r="DA4" s="92"/>
-      <c r="DB4" s="92"/>
-      <c r="DC4" s="92">
+      <c r="CW4" s="89"/>
+      <c r="CX4" s="89"/>
+      <c r="CY4" s="89"/>
+      <c r="CZ4" s="89"/>
+      <c r="DA4" s="89"/>
+      <c r="DB4" s="89"/>
+      <c r="DC4" s="89">
         <f>DC5</f>
         <v>45418</v>
       </c>
-      <c r="DD4" s="92"/>
-      <c r="DE4" s="92"/>
-      <c r="DF4" s="92"/>
-      <c r="DG4" s="92"/>
-      <c r="DH4" s="92"/>
-      <c r="DI4" s="92"/>
-      <c r="DJ4" s="89">
+      <c r="DD4" s="89"/>
+      <c r="DE4" s="89"/>
+      <c r="DF4" s="89"/>
+      <c r="DG4" s="89"/>
+      <c r="DH4" s="89"/>
+      <c r="DI4" s="89"/>
+      <c r="DJ4" s="90">
         <f>DJ5</f>
         <v>45425</v>
       </c>
-      <c r="DK4" s="90"/>
-      <c r="DL4" s="90"/>
-      <c r="DM4" s="90"/>
-      <c r="DN4" s="90"/>
-      <c r="DO4" s="90"/>
-      <c r="DP4" s="91"/>
-      <c r="DQ4" s="89">
+      <c r="DK4" s="97"/>
+      <c r="DL4" s="97"/>
+      <c r="DM4" s="97"/>
+      <c r="DN4" s="97"/>
+      <c r="DO4" s="97"/>
+      <c r="DP4" s="98"/>
+      <c r="DQ4" s="90">
         <f>DQ5</f>
         <v>45432</v>
       </c>
-      <c r="DR4" s="90"/>
-      <c r="DS4" s="90"/>
-      <c r="DT4" s="90"/>
-      <c r="DU4" s="90"/>
-      <c r="DV4" s="90"/>
-      <c r="DW4" s="91"/>
-      <c r="DX4" s="89">
+      <c r="DR4" s="97"/>
+      <c r="DS4" s="97"/>
+      <c r="DT4" s="97"/>
+      <c r="DU4" s="97"/>
+      <c r="DV4" s="97"/>
+      <c r="DW4" s="98"/>
+      <c r="DX4" s="90">
         <f>DX5</f>
         <v>45439</v>
       </c>
-      <c r="DY4" s="90"/>
-      <c r="DZ4" s="90"/>
-      <c r="EA4" s="90"/>
-      <c r="EB4" s="90"/>
-      <c r="EC4" s="90"/>
-      <c r="ED4" s="91"/>
-      <c r="EE4" s="89">
+      <c r="DY4" s="97"/>
+      <c r="DZ4" s="97"/>
+      <c r="EA4" s="97"/>
+      <c r="EB4" s="97"/>
+      <c r="EC4" s="97"/>
+      <c r="ED4" s="98"/>
+      <c r="EE4" s="90">
         <f>EE5</f>
         <v>45446</v>
       </c>
-      <c r="EF4" s="90"/>
-      <c r="EG4" s="90"/>
-      <c r="EH4" s="90"/>
-      <c r="EI4" s="90"/>
-      <c r="EJ4" s="90"/>
-      <c r="EK4" s="91"/>
-      <c r="EL4" s="89">
+      <c r="EF4" s="97"/>
+      <c r="EG4" s="97"/>
+      <c r="EH4" s="97"/>
+      <c r="EI4" s="97"/>
+      <c r="EJ4" s="97"/>
+      <c r="EK4" s="98"/>
+      <c r="EL4" s="90">
         <f>EL5</f>
         <v>45453</v>
       </c>
-      <c r="EM4" s="90"/>
-      <c r="EN4" s="90"/>
-      <c r="EO4" s="90"/>
-      <c r="EP4" s="90"/>
-      <c r="EQ4" s="90"/>
-      <c r="ER4" s="91"/>
-      <c r="ES4" s="89">
+      <c r="EM4" s="97"/>
+      <c r="EN4" s="97"/>
+      <c r="EO4" s="97"/>
+      <c r="EP4" s="97"/>
+      <c r="EQ4" s="97"/>
+      <c r="ER4" s="98"/>
+      <c r="ES4" s="90">
         <f>ES5</f>
         <v>45460</v>
       </c>
-      <c r="ET4" s="90"/>
-      <c r="EU4" s="90"/>
-      <c r="EV4" s="90"/>
-      <c r="EW4" s="90"/>
-      <c r="EX4" s="90"/>
-      <c r="EY4" s="91"/>
-      <c r="EZ4" s="89">
+      <c r="ET4" s="97"/>
+      <c r="EU4" s="97"/>
+      <c r="EV4" s="97"/>
+      <c r="EW4" s="97"/>
+      <c r="EX4" s="97"/>
+      <c r="EY4" s="98"/>
+      <c r="EZ4" s="90">
         <f>EZ5</f>
         <v>45467</v>
       </c>
-      <c r="FA4" s="90"/>
-      <c r="FB4" s="90"/>
-      <c r="FC4" s="90"/>
-      <c r="FD4" s="90"/>
-      <c r="FE4" s="90"/>
-      <c r="FF4" s="91"/>
+      <c r="FA4" s="97"/>
+      <c r="FB4" s="97"/>
+      <c r="FC4" s="97"/>
+      <c r="FD4" s="97"/>
+      <c r="FE4" s="97"/>
+      <c r="FF4" s="98"/>
     </row>
     <row r="5" spans="1:162" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="94"/>
-      <c r="B5" s="95" t="s">
+      <c r="A5" s="99"/>
+      <c r="B5" s="100" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="97" t="s">
+      <c r="C5" s="102" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="99" t="s">
+      <c r="D5" s="91" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="99" t="s">
+      <c r="E5" s="91" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="99" t="s">
+      <c r="F5" s="91" t="s">
         <v>3</v>
       </c>
       <c r="I5" s="25">
@@ -3243,12 +2922,12 @@
       </c>
     </row>
     <row r="6" spans="1:162" s="20" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="94"/>
-      <c r="B6" s="96"/>
-      <c r="C6" s="98"/>
-      <c r="D6" s="98"/>
-      <c r="E6" s="98"/>
-      <c r="F6" s="98"/>
+      <c r="A6" s="99"/>
+      <c r="B6" s="101"/>
+      <c r="C6" s="92"/>
+      <c r="D6" s="92"/>
+      <c r="E6" s="92"/>
+      <c r="F6" s="92"/>
       <c r="I6" s="28" t="str">
         <f t="shared" ref="I6:AN6" si="70">LEFT(TEXT(I5,"ddd"),1)</f>
         <v>M</v>
@@ -11750,7 +11429,7 @@
         <v>23</v>
       </c>
       <c r="D54" s="42">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="E54" s="43">
         <v>45329</v>
@@ -12278,7 +11957,7 @@
         <v>23</v>
       </c>
       <c r="D57" s="42">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="E57" s="43">
         <v>45329</v>
@@ -12625,7 +12304,7 @@
         <v>0.15</v>
       </c>
       <c r="E59" s="64">
-        <f>Project_Start</f>
+        <f t="shared" ref="E59:E70" si="115">Project_Start</f>
         <v>45329</v>
       </c>
       <c r="F59" s="64">
@@ -12802,7 +12481,7 @@
         <v>0.1</v>
       </c>
       <c r="E60" s="64">
-        <f>Project_Start</f>
+        <f t="shared" si="115"/>
         <v>45329</v>
       </c>
       <c r="F60" s="64">
@@ -12976,7 +12655,7 @@
         <v>0.95</v>
       </c>
       <c r="E61" s="64">
-        <f>Project_Start</f>
+        <f t="shared" si="115"/>
         <v>45329</v>
       </c>
       <c r="F61" s="64">
@@ -13150,7 +12829,7 @@
         <v>1</v>
       </c>
       <c r="E62" s="64">
-        <f>Project_Start</f>
+        <f t="shared" si="115"/>
         <v>45329</v>
       </c>
       <c r="F62" s="64">
@@ -13324,7 +13003,7 @@
         <v>0</v>
       </c>
       <c r="E63" s="64">
-        <f>Project_Start</f>
+        <f t="shared" si="115"/>
         <v>45329</v>
       </c>
       <c r="F63" s="64">
@@ -13498,7 +13177,7 @@
         <v>0.4</v>
       </c>
       <c r="E64" s="64">
-        <f>Project_Start</f>
+        <f t="shared" si="115"/>
         <v>45329</v>
       </c>
       <c r="F64" s="64">
@@ -13675,7 +13354,7 @@
         <v>0.85</v>
       </c>
       <c r="E65" s="64">
-        <f>Project_Start</f>
+        <f t="shared" si="115"/>
         <v>45329</v>
       </c>
       <c r="F65" s="64">
@@ -13849,7 +13528,7 @@
         <v>0</v>
       </c>
       <c r="E66" s="64">
-        <f>Project_Start</f>
+        <f t="shared" si="115"/>
         <v>45329</v>
       </c>
       <c r="F66" s="64">
@@ -14026,7 +13705,7 @@
         <v>0.9</v>
       </c>
       <c r="E67" s="64">
-        <f>Project_Start</f>
+        <f t="shared" si="115"/>
         <v>45329</v>
       </c>
       <c r="F67" s="64">
@@ -14200,7 +13879,7 @@
         <v>0</v>
       </c>
       <c r="E68" s="64">
-        <f>Project_Start</f>
+        <f t="shared" si="115"/>
         <v>45329</v>
       </c>
       <c r="F68" s="64">
@@ -14377,7 +14056,7 @@
         <v>0</v>
       </c>
       <c r="E69" s="64">
-        <f>Project_Start</f>
+        <f t="shared" si="115"/>
         <v>45329</v>
       </c>
       <c r="F69" s="64">
@@ -14554,7 +14233,7 @@
         <v>0.2</v>
       </c>
       <c r="E70" s="64">
-        <f>Project_Start</f>
+        <f t="shared" si="115"/>
         <v>45329</v>
       </c>
       <c r="F70" s="64">
@@ -15417,29 +15096,6 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="BF4:BL4"/>
-    <mergeCell ref="P4:V4"/>
-    <mergeCell ref="W4:AC4"/>
-    <mergeCell ref="AD4:AJ4"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
-    <mergeCell ref="AY4:BE4"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="Q2:Z2"/>
-    <mergeCell ref="Q1:Z1"/>
-    <mergeCell ref="I1:O1"/>
-    <mergeCell ref="I2:O2"/>
-    <mergeCell ref="I4:O4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="BM4:BS4"/>
-    <mergeCell ref="BT4:BZ4"/>
-    <mergeCell ref="CA4:CG4"/>
-    <mergeCell ref="CH4:CN4"/>
-    <mergeCell ref="CO4:CU4"/>
     <mergeCell ref="EE4:EK4"/>
     <mergeCell ref="EL4:ER4"/>
     <mergeCell ref="ES4:EY4"/>
@@ -15449,6 +15105,29 @@
     <mergeCell ref="DJ4:DP4"/>
     <mergeCell ref="DQ4:DW4"/>
     <mergeCell ref="DX4:ED4"/>
+    <mergeCell ref="BM4:BS4"/>
+    <mergeCell ref="BT4:BZ4"/>
+    <mergeCell ref="CA4:CG4"/>
+    <mergeCell ref="CH4:CN4"/>
+    <mergeCell ref="CO4:CU4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="Q2:Z2"/>
+    <mergeCell ref="Q1:Z1"/>
+    <mergeCell ref="I1:O1"/>
+    <mergeCell ref="I2:O2"/>
+    <mergeCell ref="I4:O4"/>
+    <mergeCell ref="BF4:BL4"/>
+    <mergeCell ref="P4:V4"/>
+    <mergeCell ref="W4:AC4"/>
+    <mergeCell ref="AD4:AJ4"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
+    <mergeCell ref="AY4:BE4"/>
   </mergeCells>
   <phoneticPr fontId="27" type="noConversion"/>
   <conditionalFormatting sqref="D7:D74">
@@ -15465,182 +15144,103 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I4:BL8 I9:FF74">
-    <cfRule type="expression" dxfId="43" priority="65">
+  <conditionalFormatting sqref="I9:FF9">
+    <cfRule type="expression" dxfId="20" priority="26" stopIfTrue="1">
+      <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I9:FF12">
+    <cfRule type="expression" dxfId="19" priority="25">
+      <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I9:FF74 I4:BL8">
+    <cfRule type="expression" dxfId="18" priority="65">
       <formula>AND(TODAY()&gt;=I$5, TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I10:FF11">
-    <cfRule type="expression" dxfId="42" priority="70">
-      <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="41" priority="71" stopIfTrue="1">
-      <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I15:FF20 I41:FF52">
-    <cfRule type="expression" dxfId="40" priority="68">
-      <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="39" priority="69" stopIfTrue="1">
-      <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I22:FF26 I59:FF70">
-    <cfRule type="expression" dxfId="38" priority="66">
-      <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="37" priority="67" stopIfTrue="1">
-      <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I74:FF74">
-    <cfRule type="expression" dxfId="36" priority="57">
-      <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="35" priority="58" stopIfTrue="1">
-      <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BM4:FF6">
-    <cfRule type="expression" dxfId="34" priority="49">
-      <formula>AND(TODAY()&gt;=BM$5, TODAY()&lt;BN$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I54:FF57">
-    <cfRule type="expression" dxfId="33" priority="43">
-      <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="32" priority="44" stopIfTrue="1">
-      <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I40:FF40">
-    <cfRule type="expression" dxfId="31" priority="41">
-      <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="30" priority="42" stopIfTrue="1">
-      <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I39:FF39">
-    <cfRule type="expression" dxfId="29" priority="39">
-      <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="28" priority="40" stopIfTrue="1">
-      <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I31:FF32">
-    <cfRule type="expression" dxfId="27" priority="35">
-      <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="26" priority="36" stopIfTrue="1">
-      <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I30:FF30">
-    <cfRule type="expression" dxfId="25" priority="33">
-      <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="24" priority="34" stopIfTrue="1">
-      <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I29:FF29">
-    <cfRule type="expression" dxfId="23" priority="31">
-      <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="22" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="71" stopIfTrue="1">
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I12:FF12">
-    <cfRule type="expression" dxfId="21" priority="27">
-      <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="20" priority="28" stopIfTrue="1">
-      <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I9:FF9">
-    <cfRule type="expression" dxfId="19" priority="25">
-      <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="18" priority="26" stopIfTrue="1">
-      <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I72:FF72">
-    <cfRule type="expression" dxfId="17" priority="23">
-      <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="16" priority="24" stopIfTrue="1">
-      <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I73:FF73">
-    <cfRule type="expression" dxfId="15" priority="21">
-      <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="14" priority="22" stopIfTrue="1">
-      <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I38:FF38">
-    <cfRule type="expression" dxfId="13" priority="19">
-      <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="12" priority="20" stopIfTrue="1">
-      <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I33:FF33">
-    <cfRule type="expression" dxfId="11" priority="17">
-      <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="10" priority="18" stopIfTrue="1">
-      <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I35:FF35">
-    <cfRule type="expression" dxfId="9" priority="15">
-      <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="8" priority="16" stopIfTrue="1">
-      <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I36:FF36">
-    <cfRule type="expression" dxfId="7" priority="13">
-      <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="6" priority="14" stopIfTrue="1">
-      <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I27:FF27">
-    <cfRule type="expression" dxfId="5" priority="5">
-      <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="4" priority="6" stopIfTrue="1">
-      <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I34:FF34">
-    <cfRule type="expression" dxfId="3" priority="3">
-      <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="2" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="28" stopIfTrue="1">
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I14:FF14">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="15" priority="2" stopIfTrue="1">
+      <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I14:FF20">
+    <cfRule type="expression" dxfId="14" priority="1">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="2" stopIfTrue="1">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I15:FF20 I41:FF52">
+    <cfRule type="expression" dxfId="13" priority="69" stopIfTrue="1">
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I22:FF27">
+    <cfRule type="expression" dxfId="12" priority="5">
+      <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I27:FF27">
+    <cfRule type="expression" dxfId="11" priority="6" stopIfTrue="1">
+      <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I29:FF36">
+    <cfRule type="expression" dxfId="10" priority="3">
+      <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="9" priority="4" stopIfTrue="1">
+      <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I38:FF40">
+    <cfRule type="expression" dxfId="8" priority="20" stopIfTrue="1">
+      <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I38:FF52">
+    <cfRule type="expression" dxfId="7" priority="19">
+      <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I54:FF57">
+    <cfRule type="expression" dxfId="6" priority="44" stopIfTrue="1">
+      <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="5" priority="43">
+      <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I59:FF70 I22:FF26">
+    <cfRule type="expression" dxfId="4" priority="67" stopIfTrue="1">
+      <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I59:FF70">
+    <cfRule type="expression" dxfId="3" priority="66">
+      <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I72:FF74">
+    <cfRule type="expression" dxfId="2" priority="22" stopIfTrue="1">
+      <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="21">
+      <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BM4:FF6">
+    <cfRule type="expression" dxfId="0" priority="49">
+      <formula>AND(TODAY()&gt;=BM$5, TODAY()&lt;BN$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="11">
@@ -15815,35 +15415,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="28" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="60f5a4f2d2b0abadcf532d48ebf9cb71">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7dd78129e6a1811f84807ad11c651531" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -16155,34 +15726,36 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A82239A0-E68C-493F-BEE6-C77FEA397FD6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2348D59-3426-404A-A0C5-6456F6613EDB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -16203,6 +15776,33 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A82239A0-E68C-493F-BEE6-C77FEA397FD6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata"/>
 </file>
</xml_diff>